<commit_message>
Removed CA1 (represented by Allocentric IO)
</commit_message>
<xml_diff>
--- a/WBRA/WBAH2017WBA.xlsx
+++ b/WBRA/WBAH2017WBA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="14960" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="14960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
   <si>
     <t>Isocortex</t>
   </si>
@@ -150,10 +150,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CA1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>BG</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -171,14 +167,6 @@
   </si>
   <si>
     <t>Motor Output</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Field CA1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>CA1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -242,8 +230,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,7 +274,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -303,6 +293,7 @@
     <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -322,6 +313,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -650,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -823,38 +815,24 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -871,10 +849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -948,14 +926,6 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -973,18 +943,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="13" width="5.1640625" customWidth="1"/>
+    <col min="1" max="12" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1016,13 +986,10 @@
         <v>32</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1032,14 +999,14 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
       <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1047,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1055,12 +1022,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1068,11 +1035,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1082,11 +1049,11 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1094,52 +1061,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>25</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Substantial change from the previous version.  e.g., Removed internal IOs from UB.  JSON is generated rather than hand-modified.
</commit_message>
<xml_diff>
--- a/WBRA/WBAH2017WBA.xlsx
+++ b/WBRA/WBAH2017WBA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="14960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3020" yWindow="280" windowWidth="14480" windowHeight="11240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Isocortex</t>
   </si>
@@ -30,10 +30,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Frontal Lobe</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -46,10 +42,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ASC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Associative Cortex</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -66,10 +58,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ODC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DVC</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -110,46 +98,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>UVQ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UVU</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UO</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UAllo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Umataro Visual What (Quod) I/O</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Umataro Visual Where (Ubi) I/O</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Umataro Visual Quod I/O</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Umataro Visual Ubi I/O</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Umataro Odometry I/O</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Umataro Allocentric I/O</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>BG</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -171,6 +119,58 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Reward Box</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Reward Generator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.FL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.FL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.ASC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.ASC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.ODC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.DVC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.VVC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex.VVC</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -230,7 +230,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -270,11 +270,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -294,6 +301,8 @@
     <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -314,6 +323,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="42" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -642,54 +653,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -697,142 +709,86 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -849,10 +805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -867,7 +823,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -875,7 +831,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -883,7 +839,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -891,42 +847,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -943,159 +867,151 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="12" width="5.1640625" customWidth="1"/>
+    <col min="1" max="9" width="5.1640625" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>12</v>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>34</v>
+      <c r="H10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Module V1 & connection FL to UB.  Hierarchy delimiter temporally changed to '#'.
</commit_message>
<xml_diff>
--- a/WBRA/WBAH2017WBA.xlsx
+++ b/WBRA/WBAH2017WBA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="280" windowWidth="14480" windowHeight="11240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4180" yWindow="0" windowWidth="19160" windowHeight="13480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Isocortex</t>
   </si>
@@ -82,14 +82,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Dorsal Visual Cortex</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Ventral Visual Cortex</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Visual What Path</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -142,36 +134,42 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Isocortex.FL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.FL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.ASC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.ASC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.ODC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.DVC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.VVC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Isocortex.VVC</t>
-    <phoneticPr fontId="1"/>
+    <t>Primary Visual Cortex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ventral Visual Cortices</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dorsal Visual Cortices</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Primary Visual Area</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isocortex#FL</t>
+  </si>
+  <si>
+    <t>Isocortex#ASC</t>
+  </si>
+  <si>
+    <t>Isocortex#ODC</t>
+  </si>
+  <si>
+    <t>Isocortex#DVC</t>
+  </si>
+  <si>
+    <t>Isocortex#VVC</t>
+  </si>
+  <si>
+    <t>Isocortex#V1</t>
   </si>
 </sst>
 </file>
@@ -230,8 +228,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -281,7 +297,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="61">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -303,6 +319,15 @@
     <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -325,6 +350,15 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -653,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -667,10 +701,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -681,10 +715,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -695,10 +729,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -709,86 +743,100 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D10" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -805,10 +853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -850,6 +898,14 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -867,150 +923,167 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="9" width="5.1640625" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" customWidth="1"/>
+    <col min="1" max="10" width="5.1640625" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="H10">
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>

</xml_diff>